<commit_message>
refactor: add report download
</commit_message>
<xml_diff>
--- a/src/db/template-item.xlsx
+++ b/src/db/template-item.xlsx
@@ -11,19 +11,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Proof Blend Coffee</t>
   </si>
   <si>
     <t>gr</t>
+  </si>
+  <si>
+    <t>Fresh Milk Green Field</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>UHT Milk Indomilk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -34,11 +43,6 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,8 +66,8 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -289,6 +293,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>